<commit_message>
Änderungen von UNI auf GIT
</commit_message>
<xml_diff>
--- a/Doku/Bauteilliste Solarregler V0.1.xlsx
+++ b/Doku/Bauteilliste Solarregler V0.1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="215">
   <si>
     <t>Lfd. Nummer</t>
   </si>
@@ -658,6 +658,63 @@
   </si>
   <si>
     <t xml:space="preserve">IE2405S oder TME2405S </t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/tracopower-tme-2405s-dcdc-wandler-print-24-vdc-5-vdc-200-ma-1-w-anzahl-ausgaenge-1-x-154477.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/finder-361190054011-printrelais-5-vdc-10-a-1-wechsler-1-st-503243.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/dip-schalter-polzahl-8-smd-apem-ikh0803000-1-st-700772.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/tvs-diode-nexperia-pesd2can215-sot-23-262-v-230-w-1096200.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/tvs-diode-bourns-smaj30ca-do-214ac-333-v-400-w-1056305.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/quarzkristall-euroquartz-quarz-tc26-zylinder-32768-khz-125-pf-o-x-h-2-mm-x-62-mm-1-st-156007.html</t>
+  </si>
+  <si>
+    <t>https://de.rs-online.com/web/p/quarzmodule/1710659/</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/panjit-schottky-diode-gleichrichter-sr36-do-214aa-60-v-einzeln-1304924.html</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>D3-1, D3-3</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/pmic-waermemanagement-maxim-integrated-max31865atp-extern-spi-tqfn-20-ep-5x5-1123421.html</t>
+  </si>
+  <si>
+    <t>https://de.rs-online.com/web/p/metalloxid-varistoren/7606961/</t>
+  </si>
+  <si>
+    <t>https://de.rs-online.com/web/p/rueckstellende-sicherungen-smd/6478342/</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/tvs-diode-stmicroelectronics-dviulc6-4sc6y-sot-23-6l-6-v-1183886.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/yageo-cc1206zpy5v7bb475-keramik-kondensator-smd-1206-47-f-16-v-20-1-st-445372.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/tantal-kondensator-smd-22-f-63-v-20-l-x-b-35-mm-x-28-mm-panasonic-6tpu22msi-1-st-1479548.html</t>
+  </si>
+  <si>
+    <t>https://de.rs-online.com/web/p/keramik-multilayer-kondensatoren/9159328/</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/microtech-cmf0603402r0110-duennschicht-widerstand-402-smd-0603-01-w-01-10-ppm-1-st-1457041.html</t>
   </si>
 </sst>
 </file>
@@ -2319,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,7 +2388,7 @@
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2350,8 +2407,11 @@
       <c r="F1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2371,7 +2431,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2391,7 +2451,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2411,7 +2471,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2431,7 +2491,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2451,7 +2511,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2471,7 +2531,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2491,7 +2551,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2511,7 +2571,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2530,8 +2590,11 @@
       <c r="F10" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2551,7 +2614,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2571,7 +2634,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2591,7 +2654,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2611,7 +2674,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2631,7 +2694,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2651,7 +2714,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2670,8 +2733,11 @@
       <c r="F17" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2690,8 +2756,11 @@
       <c r="F18" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2710,8 +2779,11 @@
       <c r="F19" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2730,8 +2802,11 @@
       <c r="F20" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2750,8 +2825,11 @@
       <c r="F21" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2759,16 +2837,19 @@
         <v>167</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>206</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2784,25 +2865,28 @@
       <c r="F23" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>168</v>
       </c>
-      <c r="D24" t="s">
-        <v>104</v>
-      </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2818,8 +2902,11 @@
       <c r="F25" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2839,7 +2926,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2856,7 +2943,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2873,7 +2960,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2889,8 +2976,11 @@
       <c r="F29" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2909,8 +2999,11 @@
       <c r="G30" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2927,7 +3020,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2943,8 +3036,11 @@
       <c r="F32" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2960,8 +3056,11 @@
       <c r="F33" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2977,8 +3076,11 @@
       <c r="F34" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2994,8 +3096,11 @@
       <c r="F35" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3012,7 +3117,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3028,8 +3133,11 @@
       <c r="F37" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3046,7 +3154,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3063,7 +3171,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>

</xml_diff>